<commit_message>
Programa e Mais alguns casos de uso
</commit_message>
<xml_diff>
--- a/descricao de casodeuso.xlsx
+++ b/descricao de casodeuso.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Engenharia-Software-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E310DD7F-21EA-48CD-934D-F78F15190CB7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61E6FD2-C2A9-45F7-AA7A-E7DF92D1D516}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Consultar Cliente" sheetId="3" r:id="rId1"/>
-    <sheet name="Editar Cliente" sheetId="2" r:id="rId2"/>
-    <sheet name="Criar Cliente" sheetId="1" r:id="rId3"/>
+    <sheet name="Criar Cliente" sheetId="1" r:id="rId1"/>
+    <sheet name="Consultar Cliente" sheetId="3" r:id="rId2"/>
+    <sheet name="Editar Cliente" sheetId="2" r:id="rId3"/>
+    <sheet name="Eliminar Cliente" sheetId="5" r:id="rId4"/>
+    <sheet name=" Ver Empregado" sheetId="6" r:id="rId5"/>
+    <sheet name=" Criar Empregado" sheetId="7" r:id="rId6"/>
+    <sheet name=" Alterar Empregado" sheetId="9" r:id="rId7"/>
+    <sheet name="Eliminar Empregado" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="62">
   <si>
     <t>nome</t>
   </si>
@@ -141,6 +146,78 @@
   </si>
   <si>
     <t>o sistema devolve uma caixa de texto para inserir o nome do cliente</t>
+  </si>
+  <si>
+    <t>Eliminar Cliente</t>
+  </si>
+  <si>
+    <t>O empregado vai apagar cliente</t>
+  </si>
+  <si>
+    <t>clicar na aba apagar cliente</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os dados do cliente com a opção para eliminar</t>
+  </si>
+  <si>
+    <t>O ator confirma que quer eliminar</t>
+  </si>
+  <si>
+    <t>verificar se o sistema guarda as alteraçoes</t>
+  </si>
+  <si>
+    <t>Visualizar Empregado</t>
+  </si>
+  <si>
+    <t>tem que existir dados do empregado</t>
+  </si>
+  <si>
+    <t>clicar na aba Controlo</t>
+  </si>
+  <si>
+    <t>Selecionar a de empregados</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os dados dos empregados</t>
+  </si>
+  <si>
+    <t>Criar Empregado</t>
+  </si>
+  <si>
+    <t>O ator vai visualizar os empregados</t>
+  </si>
+  <si>
+    <t>O Chefe vai criar um empregado</t>
+  </si>
+  <si>
+    <t>Selecionar a de criar empregados</t>
+  </si>
+  <si>
+    <t>O ator preenche os dados e confirma</t>
+  </si>
+  <si>
+    <t>verificar se o sistema guarda as informações</t>
+  </si>
+  <si>
+    <t>o ator altera os dados que pretende e clica no confirmar</t>
+  </si>
+  <si>
+    <t>O Chefe vai alterar um empregado</t>
+  </si>
+  <si>
+    <t>Alterar Empregado</t>
+  </si>
+  <si>
+    <t>Eliminar Empregado</t>
+  </si>
+  <si>
+    <t>O Chefe vai eliminar um empregado</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os dados do empregado</t>
+  </si>
+  <si>
+    <t>O ator confirma que quer apagar</t>
   </si>
 </sst>
 </file>
@@ -613,10 +690,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67AE3C0-BE48-44F0-8898-2D5C99120618}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -789,7 +1039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32040F67-D8CC-4C9B-B010-54A4C3AE0575}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -972,12 +1222,195 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DECE30A-1DD4-46EC-AF00-7092D6283564}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36CEA24-EAE0-46DF-8602-76CDA3E70D48}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B6" sqref="B6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,14 +1442,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1029,20 +1464,24 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -1097,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,20 +1548,543 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D14257-1547-495C-A2D4-7EBB725458EA}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A6D37C-768B-40A3-A424-1C7437DC6CAD}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D00E3-DD36-49C9-B4B0-089B3E9A56B9}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
atualização do git hub
</commit_message>
<xml_diff>
--- a/descricao de casodeuso.xlsx
+++ b/descricao de casodeuso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Engenharia-Software-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61E6FD2-C2A9-45F7-AA7A-E7DF92D1D516}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF2E44D-25F2-4EAC-93CA-C2C81B317D01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" tabRatio="844" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Criar Cliente" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,12 @@
     <sheet name=" Criar Empregado" sheetId="7" r:id="rId6"/>
     <sheet name=" Alterar Empregado" sheetId="9" r:id="rId7"/>
     <sheet name="Eliminar Empregado" sheetId="10" r:id="rId8"/>
+    <sheet name="Criar Compra" sheetId="14" r:id="rId9"/>
+    <sheet name="Alterar Compra " sheetId="15" r:id="rId10"/>
+    <sheet name="Consultar Compra" sheetId="16" r:id="rId11"/>
+    <sheet name="Criar Arranjo" sheetId="17" r:id="rId12"/>
+    <sheet name="Alterar Arranjo" sheetId="18" r:id="rId13"/>
+    <sheet name="Consultar Arranjo" sheetId="19" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="102">
   <si>
     <t>nome</t>
   </si>
@@ -218,6 +224,126 @@
   </si>
   <si>
     <t>O ator confirma que quer apagar</t>
+  </si>
+  <si>
+    <t>Criar Compra</t>
+  </si>
+  <si>
+    <t>O Ator vai criar uma compra</t>
+  </si>
+  <si>
+    <t>Tem que existir um cliente criado</t>
+  </si>
+  <si>
+    <t>clicar na aba Compra</t>
+  </si>
+  <si>
+    <t>Selecionar a de criar compra</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os artigos</t>
+  </si>
+  <si>
+    <t>O ator seleciona os artigos e confirma</t>
+  </si>
+  <si>
+    <t>O sistema guarda os artigos na compra criada</t>
+  </si>
+  <si>
+    <t>Alterar Compra</t>
+  </si>
+  <si>
+    <t>O Ator vai alterar uma compra</t>
+  </si>
+  <si>
+    <t>Tem que existir uma compra criada</t>
+  </si>
+  <si>
+    <t>Selecionar a de alterar compra</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os artigos dessa compra</t>
+  </si>
+  <si>
+    <t>O sistema guarda as alteraçoes</t>
+  </si>
+  <si>
+    <t>O ator faz as alteraçoes e confirma</t>
+  </si>
+  <si>
+    <t>Consultar Compra</t>
+  </si>
+  <si>
+    <t>O Ator vai consultar uma compra</t>
+  </si>
+  <si>
+    <t>Selecionar a de ver compra</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com o id da compra</t>
+  </si>
+  <si>
+    <t>O ator seleciona o id da compra e confirma</t>
+  </si>
+  <si>
+    <t>O sistema devolve a compra com os respectivos artigos</t>
+  </si>
+  <si>
+    <t>Criar Arranjo</t>
+  </si>
+  <si>
+    <t>O Ator vai criar um arranjo</t>
+  </si>
+  <si>
+    <t>Tem que existir um cliente</t>
+  </si>
+  <si>
+    <t>clicar na aba Arranjo</t>
+  </si>
+  <si>
+    <t>Selecionar a criar Arranjo</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario para criar o arranjo</t>
+  </si>
+  <si>
+    <t>O ator escreve os dados do arranjo e confirma</t>
+  </si>
+  <si>
+    <t>O sistema guarda os dados do arranjo</t>
+  </si>
+  <si>
+    <t>Alterar Arranjo</t>
+  </si>
+  <si>
+    <t>O Ator vai alterar um arranjo</t>
+  </si>
+  <si>
+    <t>Tem que existir um arranjo</t>
+  </si>
+  <si>
+    <t>Selecionar a de alterar Arranjo</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma caixa de texto para inserir o id do arranjo</t>
+  </si>
+  <si>
+    <t>O ator escreve o id do arranjo e confirma</t>
+  </si>
+  <si>
+    <t>O sistema devolve o formulário com os dados do arranjo do id selecionado</t>
+  </si>
+  <si>
+    <t>O ator faz as respetivas alteraçoes e confirma</t>
+  </si>
+  <si>
+    <t>Consultar Arranjo</t>
+  </si>
+  <si>
+    <t>O Ator vai consultar um arranjo</t>
+  </si>
+  <si>
+    <t>Selecionar a de Consultar Arranjo</t>
   </si>
 </sst>
 </file>
@@ -862,6 +988,929 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BF4339-F1E5-468C-8BEC-092D00FC786A}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D6964B-83F2-4E15-841F-4595B43CF748}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA05E02-7A43-48BB-BA47-2B0C293579E9}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F56D77-C4EB-43F5-B1EA-1703A8794010}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7958BD0D-A262-48DA-996D-F790BF03E7CB}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67AE3C0-BE48-44F0-8898-2D5C99120618}">
   <dimension ref="A1:B23"/>
@@ -1934,7 +2983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D00E3-DD36-49C9-B4B0-089B3E9A56B9}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2105,4 +3154,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE2EFA7-0EA2-45E2-A8F6-14BE443FC966}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>